<commit_message>
new deleted file log and change some configurations
</commit_message>
<xml_diff>
--- a/svcEngine/bin/dataset/dataset.xlsx
+++ b/svcEngine/bin/dataset/dataset.xlsx
@@ -8,29 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\TMMIN Project\opcua_client_service\svcEngine\bin\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07A81D8-003F-4591-9E6F-1AF65FB3D042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FB4089-23BD-401C-87D1-EF09C81127D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>009</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>000</t>
   </si>
   <si>
-    <t>002</t>
-  </si>
-  <si>
     <t>ASSET_ID</t>
   </si>
   <si>
@@ -49,19 +56,10 @@
     <t>INDEX_LIST_VALUE</t>
   </si>
   <si>
-    <t>ns=2;s=PLC_ST_2.400943320700103000-000-009-5633</t>
-  </si>
-  <si>
-    <t>ns=2;s=KWS_2_3.400943320700103003-002-000-5002</t>
-  </si>
-  <si>
-    <t>400943320700103003</t>
-  </si>
-  <si>
-    <t>400943320700103000</t>
-  </si>
-  <si>
-    <t>003, 004, 005, 006, 007, 008</t>
+    <t>4009433100000000000000</t>
+  </si>
+  <si>
+    <t>ns=2;s=PC10.test blink</t>
   </si>
 </sst>
 </file>
@@ -97,9 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,72 +402,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
+      <c r="A2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>5002</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>5633</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>